<commit_message>
Se agregan tiempo de ejecucion de recursividad par
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PrograAvanzada\Proyectos en GitHub\TPOrganizacion\PolinomiosGrupal\PruebasParaElTP2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -92,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,17 +258,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -282,7 +267,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -305,14 +290,23 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -320,34 +314,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -371,7 +343,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -411,7 +382,7 @@
                   <c:v>34341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>70132</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20921</c:v>
@@ -455,7 +426,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -495,7 +465,7 @@
                   <c:v>104208</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>95791</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6710</c:v>
@@ -539,7 +509,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -579,7 +548,7 @@
                   <c:v>48157</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>595270</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20131</c:v>
@@ -600,28 +569,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:gapWidth val="182"/>
-        <c:axId val="321236128"/>
-        <c:axId val="321237808"/>
+        <c:axId val="70861568"/>
+        <c:axId val="70863104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="321236128"/>
+        <c:axId val="70861568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -641,7 +601,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -653,22 +613,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321237808"/>
+        <c:crossAx val="70863104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321237808"/>
+        <c:axId val="70863104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -686,7 +644,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -700,7 +657,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -712,10 +669,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321236128"/>
+        <c:crossAx val="70861568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,7 +687,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -743,7 +699,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -755,13 +711,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -785,12 +740,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1419,7 +1374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1454,7 +1409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1631,28 +1586,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1674,7 +1629,7 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1692,7 +1647,7 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1710,7 +1665,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1732,7 +1687,7 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1778,7 +1733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1800,7 +1755,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1822,7 +1777,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1844,7 +1799,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1866,7 +1821,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1888,7 +1843,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1910,7 +1865,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1928,7 +1883,7 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1946,7 +1901,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
         <v>5</v>
@@ -1992,7 +1947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -2028,7 +1983,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -2051,7 +2006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2059,7 +2014,7 @@
         <v>34341</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>70132</v>
       </c>
       <c r="D21">
         <v>20921</v>
@@ -2077,7 +2032,7 @@
         <v>25263</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2085,7 +2040,7 @@
         <v>104208</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>95791</v>
       </c>
       <c r="D22">
         <v>6710</v>
@@ -2103,7 +2058,7 @@
         <v>35526</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2111,7 +2066,7 @@
         <v>48157</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>595270</v>
       </c>
       <c r="D23">
         <v>20131</v>

</xml_diff>

<commit_message>
Se agrega a Binomio de Newton Horner y Programacion Dinamica
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceYanina\PruebasParaElTP2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11025"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -87,8 +92,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +244,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,7 +264,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -342,6 +358,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -350,11 +367,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -378,6 +397,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -461,6 +481,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -544,6 +565,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -604,18 +626,28 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="78613120"/>
-        <c:axId val="78627200"/>
+        <c:axId val="337567112"/>
+        <c:axId val="337568288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78613120"/>
+        <c:axId val="337567112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -647,20 +679,22 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78627200"/>
+        <c:crossAx val="337568288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78627200"/>
+        <c:axId val="337568288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -678,6 +712,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -703,10 +738,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78613120"/>
+        <c:crossAx val="337567112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -721,6 +756,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -745,12 +781,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -774,7 +811,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -787,7 +824,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -809,7 +856,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="es-ES"/>
               <a:t>Tiempo de Resolucion en NanoSegundos
 BINOMIO</a:t>
             </a:r>
@@ -829,7 +876,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="es-ES"/>
               <a:t>
 </a:t>
             </a:r>
@@ -844,6 +891,7 @@
           <c:y val="9.9378869026736563E-3"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -852,11 +900,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -871,6 +921,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$K$20:$Q$20</c:f>
@@ -911,6 +962,12 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5249</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2094</c:v>
@@ -936,6 +993,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$K$20:$Q$20</c:f>
@@ -976,6 +1034,12 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>29324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>652688</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17148</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1746</c:v>
@@ -1001,6 +1065,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$K$20:$Q$20</c:f>
@@ -1042,6 +1107,12 @@
                 <c:pt idx="1">
                   <c:v>352932</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>1028901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43745</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>15360</c:v>
                 </c:pt>
@@ -1052,18 +1123,28 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="50956160"/>
-        <c:axId val="50957696"/>
+        <c:axId val="337567896"/>
+        <c:axId val="337569072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50956160"/>
+        <c:axId val="337567896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1095,20 +1176,22 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50957696"/>
+        <c:crossAx val="337569072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50957696"/>
+        <c:axId val="337569072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1126,6 +1209,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1151,10 +1235,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50956160"/>
+        <c:crossAx val="337567896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1169,6 +1253,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1193,12 +1278,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1222,7 +1308,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1553,28 +1639,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1682,7 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1614,7 +1700,7 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1632,7 +1718,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1654,7 +1740,7 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1700,7 +1786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1722,7 +1808,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1744,7 +1830,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1766,7 +1852,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1874,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1810,7 +1896,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1832,7 +1918,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1850,7 +1936,7 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1868,7 +1954,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
         <v>5</v>
@@ -1914,7 +2000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1950,7 +2036,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1994,7 +2080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2028,6 +2114,12 @@
       <c r="L21">
         <v>11869</v>
       </c>
+      <c r="M21">
+        <v>51096</v>
+      </c>
+      <c r="N21">
+        <v>5249</v>
+      </c>
       <c r="P21">
         <v>2094</v>
       </c>
@@ -2035,7 +2127,7 @@
         <v>2444</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2069,6 +2161,12 @@
       <c r="L22">
         <v>29324</v>
       </c>
+      <c r="M22" s="9">
+        <v>652688</v>
+      </c>
+      <c r="N22">
+        <v>17148</v>
+      </c>
       <c r="P22">
         <v>1746</v>
       </c>
@@ -2076,7 +2174,7 @@
         <v>2444</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2109,6 +2207,12 @@
       </c>
       <c r="L23">
         <v>352932</v>
+      </c>
+      <c r="M23">
+        <v>1028901</v>
+      </c>
+      <c r="N23">
+        <v>43745</v>
       </c>
       <c r="P23">
         <v>15360</v>

</xml_diff>

<commit_message>
Se agrega complejidad computacional de los binomios en el excel
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceYanina\PruebasParaElTP2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11025"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
   <si>
     <t>Grado 0</t>
   </si>
@@ -92,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -244,7 +240,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,17 +259,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -358,7 +343,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -367,13 +351,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -397,7 +379,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -481,7 +462,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -565,7 +545,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$20:$H$20</c:f>
@@ -626,28 +605,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:gapWidth val="182"/>
-        <c:axId val="337567112"/>
-        <c:axId val="337568288"/>
+        <c:axId val="67461888"/>
+        <c:axId val="67463424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="337567112"/>
+        <c:axId val="67461888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -679,22 +649,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337568288"/>
+        <c:crossAx val="67463424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337568288"/>
+        <c:axId val="67463424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -712,7 +680,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -738,10 +705,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337567112"/>
+        <c:crossAx val="67461888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -756,7 +723,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -781,13 +747,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -811,12 +776,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -824,17 +789,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -888,10 +843,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.28645303738146932"/>
-          <c:y val="9.9378869026736563E-3"/>
+          <c:y val="9.937886902673658E-3"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -900,13 +854,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -921,7 +873,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$K$20:$Q$20</c:f>
@@ -993,7 +944,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$K$20:$Q$20</c:f>
@@ -1065,7 +1015,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$K$20:$Q$20</c:f>
@@ -1123,28 +1072,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:gapWidth val="182"/>
-        <c:axId val="337567896"/>
-        <c:axId val="337569072"/>
+        <c:axId val="69493504"/>
+        <c:axId val="69495040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="337567896"/>
+        <c:axId val="69493504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1176,22 +1116,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337569072"/>
+        <c:crossAx val="69495040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337569072"/>
+        <c:axId val="69495040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1209,7 +1147,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1235,10 +1172,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337567896"/>
+        <c:crossAx val="69493504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1253,7 +1190,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1278,13 +1214,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1308,12 +1243,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1639,108 +1574,108 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+    <row r="3" spans="1:17">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:17">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="8" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1786,7 +1721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1808,7 +1743,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1830,7 +1765,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1852,7 +1787,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1874,7 +1809,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1896,65 +1831,65 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:17">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="J11" s="6" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="J11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+    <row r="12" spans="1:17">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+    <row r="13" spans="1:17">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
         <v>5</v>
@@ -2000,7 +1935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -2028,15 +1963,27 @@
       <c r="J15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
@@ -2080,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2127,7 +2074,7 @@
         <v>2444</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2161,7 +2108,7 @@
       <c r="L22">
         <v>29324</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="6">
         <v>652688</v>
       </c>
       <c r="N22">
@@ -2174,7 +2121,7 @@
         <v>2444</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de los test
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceYanina\PruebasParaElTP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanina\Documents\UnLaM\PrograAvanzada2017\workspace\PruebasParaElTP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
   <si>
     <t>Grado 0</t>
   </si>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,6 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -244,7 +245,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -357,7 +357,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -404,25 +403,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Recursiva</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>RecursivaPar</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Horner</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>ProgDinam</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mejorado</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Pow</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Msucesiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -434,29 +433,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>25263</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>34341</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>70132</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>20921</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>19341</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>17763</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>46973</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74CC-48A0-BF49-B41158BA660B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -488,25 +492,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Recursiva</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>RecursivaPar</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Horner</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>ProgDinam</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mejorado</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Pow</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Msucesiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -518,29 +522,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>35526</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>104208</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>95791</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6710</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5132</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5921</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32368</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-74CC-48A0-BF49-B41158BA660B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -572,25 +581,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Recursiva</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>RecursivaPar</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Horner</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>ProgDinam</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mejorado</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Pow</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Msucesiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -602,29 +611,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>105392</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>48157</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>595270</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>20131</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>19737</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16184</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>29605</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-74CC-48A0-BF49-B41158BA660B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -635,11 +649,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="337567112"/>
-        <c:axId val="337568288"/>
+        <c:axId val="67461888"/>
+        <c:axId val="67463424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="337567112"/>
+        <c:axId val="67461888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,10 +693,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337568288"/>
+        <c:crossAx val="67463424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -690,7 +704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337568288"/>
+        <c:axId val="67463424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,10 +752,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337567112"/>
+        <c:crossAx val="67461888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -755,7 +769,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -781,7 +794,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -811,19 +824,19 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -888,7 +901,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.28645303738146932"/>
-          <c:y val="9.9378869026736563E-3"/>
+          <c:y val="9.937886902673658E-3"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -928,25 +941,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Recursiva</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>RecursivaPar</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Horner</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>ProgDinam</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mejorado</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Pow</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Msucesiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -958,26 +971,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>2444</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7331</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>11869</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>51096</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5249</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2094</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF98-4BBA-AB58-CE0DB2692DE2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1000,25 +1018,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Recursiva</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>RecursivaPar</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Horner</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>ProgDinam</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mejorado</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Pow</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Msucesiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1030,26 +1048,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>2444</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>20946</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>29324</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>652688</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>17148</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1746</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EF98-4BBA-AB58-CE0DB2692DE2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1072,25 +1095,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Recursiva</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>RecursivaPar</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Horner</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>ProgDinam</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mejorado</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Pow</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Msucesiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1102,26 +1125,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>12567</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>504787</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>352932</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1028901</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43745</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>15360</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12567</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EF98-4BBA-AB58-CE0DB2692DE2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1132,11 +1160,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="337567896"/>
-        <c:axId val="337569072"/>
+        <c:axId val="69493504"/>
+        <c:axId val="69495040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="337567896"/>
+        <c:axId val="69493504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,10 +1204,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337569072"/>
+        <c:crossAx val="69495040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1187,7 +1215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337569072"/>
+        <c:axId val="69495040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,10 +1263,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337567896"/>
+        <c:crossAx val="69493504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1252,7 +1280,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1278,7 +1305,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1308,12 +1335,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1336,7 +1363,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1366,7 +1399,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 1"/>
+        <xdr:cNvPr id="4" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1649,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,84 +1700,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="8" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -1897,62 +1936,62 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="J11" s="6" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="J11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -2028,56 +2067,68 @@
       <c r="J15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="O20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="P20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="Q20" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2085,46 +2136,46 @@
         <v>3</v>
       </c>
       <c r="B21">
+        <v>25263</v>
+      </c>
+      <c r="C21">
         <v>34341</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>70132</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>20921</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>19341</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>17763</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>46973</v>
-      </c>
-      <c r="H21">
-        <v>25263</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K21">
+        <v>2444</v>
+      </c>
+      <c r="L21">
         <v>7331</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>11869</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>51096</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>5249</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>2094</v>
-      </c>
-      <c r="Q21">
-        <v>2444</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2132,46 +2183,46 @@
         <v>19</v>
       </c>
       <c r="B22">
+        <v>35526</v>
+      </c>
+      <c r="C22">
         <v>104208</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>95791</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>6710</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>5132</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>5921</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>32368</v>
-      </c>
-      <c r="H22">
-        <v>35526</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K22">
+        <v>2444</v>
+      </c>
+      <c r="L22">
         <v>20946</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>29324</v>
       </c>
-      <c r="M22" s="9">
+      <c r="N22" s="6">
         <v>652688</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>17148</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>1746</v>
-      </c>
-      <c r="Q22">
-        <v>2444</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2179,46 +2230,46 @@
         <v>20</v>
       </c>
       <c r="B23">
+        <v>105392</v>
+      </c>
+      <c r="C23">
         <v>48157</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>595270</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>20131</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>19737</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>16184</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>29605</v>
-      </c>
-      <c r="H23">
-        <v>105392</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K23">
+        <v>12567</v>
+      </c>
+      <c r="L23">
         <v>504787</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>352932</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>1028901</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>43745</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>15360</v>
-      </c>
-      <c r="Q23">
-        <v>12567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega evaluarMejorada para Binomio de Newton
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
   <si>
     <t>Grado 0</t>
   </si>
@@ -88,12 +88,15 @@
   <si>
     <t>Grado 100</t>
   </si>
+  <si>
+    <t>n/2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +130,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -218,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,6 +256,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,6 +997,9 @@
                 <c:pt idx="4">
                   <c:v>5249</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>4619</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>2094</c:v>
                 </c:pt>
@@ -1062,6 +1077,9 @@
                 <c:pt idx="4">
                   <c:v>17148</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>5132</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1746</c:v>
                 </c:pt>
@@ -1138,6 +1156,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43745</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21553</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>15360</c:v>
@@ -1686,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,12 +2103,14 @@
       <c r="O15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P15" s="1"/>
+      <c r="P15" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="Q15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
@@ -2131,7 +2154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2174,11 +2197,14 @@
       <c r="O21">
         <v>5249</v>
       </c>
+      <c r="P21">
+        <v>4619</v>
+      </c>
       <c r="Q21">
         <v>2094</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2221,11 +2247,14 @@
       <c r="O22">
         <v>17148</v>
       </c>
+      <c r="P22">
+        <v>5132</v>
+      </c>
       <c r="Q22">
         <v>1746</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2268,9 +2297,15 @@
       <c r="O23">
         <v>43745</v>
       </c>
+      <c r="P23">
+        <v>21553</v>
+      </c>
       <c r="Q23">
         <v>15360</v>
       </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Se agrega Desarrollo de Binomio para Msucesivas
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -5,14 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PrograAvanzada\Proyectos en GitHub\TPOrganizacion\PolinomiosGrupal\PruebasParaElTP2\PruebasParaElTP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceYanina\PruebasParaElTP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="POLINOMIO" sheetId="1" r:id="rId1"/>
+    <sheet name="BINOMIO DE NEWTON" sheetId="2" r:id="rId2"/>
+    <sheet name="BINOMIO DE NEWTON DESARROLLADO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="24">
   <si>
     <t>Grado 0</t>
   </si>
@@ -285,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,15 +305,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,6 +321,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +472,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$A$23</c:f>
+              <c:f>POLINOMIO!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -485,7 +493,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$22:$H$22</c:f>
+              <c:f>POLINOMIO!$B$22:$H$22</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -514,7 +522,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$23:$H$23</c:f>
+              <c:f>POLINOMIO!$B$23:$H$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -553,7 +561,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$A$24</c:f>
+              <c:f>POLINOMIO!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -574,7 +582,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$22:$H$22</c:f>
+              <c:f>POLINOMIO!$B$22:$H$22</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -603,7 +611,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$24:$H$24</c:f>
+              <c:f>POLINOMIO!$B$24:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -642,7 +650,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$A$25</c:f>
+              <c:f>POLINOMIO!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -663,7 +671,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$22:$H$22</c:f>
+              <c:f>POLINOMIO!$B$22:$H$22</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -692,7 +700,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$25:$H$25</c:f>
+              <c:f>POLINOMIO!$B$25:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -735,11 +743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="194841488"/>
-        <c:axId val="194845968"/>
+        <c:axId val="331190056"/>
+        <c:axId val="331196328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="194841488"/>
+        <c:axId val="331190056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,7 +790,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194845968"/>
+        <c:crossAx val="331196328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194845968"/>
+        <c:axId val="331196328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,7 +849,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194841488"/>
+        <c:crossAx val="331190056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,6 +951,455 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>Diferencias entre Horner </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+              <a:t> con desarrollo del polinomio y Programación dinámica evaluado de forma directa</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14288188976377952"/>
+          <c:y val="4.6296296296296294E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>POLINOMIO!$U$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ProgDinam</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>POLINOMIO!$T$23:$T$25</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Grado 20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Grado 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Grado 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>POLINOMIO!$U$23:$U$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5249</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43745</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>POLINOMIO!$V$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>POLINOMIO!$T$23:$T$25</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Grado 20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Grado 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Grado 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>POLINOMIO!$V$23:$V$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>51096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>652688</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1028901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="331194368"/>
+        <c:axId val="331194760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="331194368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331194760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="331194760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331194368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -1012,7 +1469,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$J$23</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1024,7 +1481,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$K$22:$Q$22</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$B$22:$H$22</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1053,7 +1510,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$K$23:$Q$23</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$B$23:$H$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1092,7 +1549,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$J$24</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1104,7 +1561,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$K$22:$Q$22</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$B$22:$H$22</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1133,7 +1590,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$K$24:$Q$24</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$B$24:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1172,7 +1629,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$J$25</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1184,7 +1641,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$K$22:$Q$22</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$B$22:$H$22</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1213,7 +1670,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$K$25:$Q$25</c:f>
+              <c:f>'BINOMIO DE NEWTON'!$B$25:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1256,11 +1713,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="189824944"/>
-        <c:axId val="189823824"/>
+        <c:axId val="381338832"/>
+        <c:axId val="381341184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189824944"/>
+        <c:axId val="381338832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1760,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189823824"/>
+        <c:crossAx val="381341184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1311,7 +1768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189823824"/>
+        <c:axId val="381341184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1819,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189824944"/>
+        <c:crossAx val="381338832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1443,7 +1900,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1464,7 +1921,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1477,14 +1934,30 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-ES" sz="1100"/>
-              <a:t>Diferencias entre Horner </a:t>
+              <a:rPr lang="es-ES"/>
+              <a:t>Tiempo de Resolucion en NanoSegundos
+BINOMIO DESARROLLADO</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-              <a:t> con desarrollo del polinomio y Programación dinámica evaluado de forma directa</a:t>
+              <a:rPr lang="es-ES"/>
+              <a:t>
+</a:t>
             </a:r>
-            <a:endParaRPr lang="es-ES" sz="1100"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1492,8 +1965,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14288188976377952"/>
-          <c:y val="4.6296296296296294E-3"/>
+          <c:x val="0.28645303738146932"/>
+          <c:y val="9.937886902673658E-3"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1504,182 +1977,199 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$U$22</c:f>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ProgDinam</c:v>
+                  <c:v>Grado 20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$T$23:$T$25</c:f>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$22:$H$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Grado 20</c:v>
+                  <c:v>Msucesiva</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Grado 50</c:v>
+                  <c:v>Recursiva</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Grado 100</c:v>
+                  <c:v>RecursivaPar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Horner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ProgDinam</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mejorado</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pow</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$U$23:$U$25</c:f>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$23:$H$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5249</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17148</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43745</c:v>
+                  <c:v>36046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF98-4BBA-AB58-CE0DB2692DE2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$V$22</c:f>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horner</c:v>
+                  <c:v>Grado 50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$T$23:$T$25</c:f>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$22:$H$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Grado 20</c:v>
+                  <c:v>Msucesiva</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Grado 50</c:v>
+                  <c:v>Recursiva</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Grado 100</c:v>
+                  <c:v>RecursivaPar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Horner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ProgDinam</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mejorado</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pow</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$V$23:$V$25</c:f>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$24:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>51096</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>652688</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1028901</c:v>
+                  <c:v>266324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EF98-4BBA-AB58-CE0DB2692DE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grado 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$22:$H$22</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Msucesiva</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Recursiva</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RecursivaPar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Horner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ProgDinam</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mejorado</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1245531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EF98-4BBA-AB58-CE0DB2692DE2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1689,30 +2179,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302595136"/>
-        <c:axId val="302602976"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="302595136"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="332302544"/>
+        <c:axId val="382465464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="332302544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1721,8 +2199,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1734,7 +2212,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1749,17 +2227,20 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302602976"/>
+        <c:crossAx val="382465464"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="302602976"/>
+        <c:axId val="382465464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1780,14 +2261,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1796,7 +2271,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1811,9 +2286,9 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302595136"/>
+        <c:crossAx val="332302544"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1839,7 +2314,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1886,7 +2361,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2468,7 +2943,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2488,26 +2963,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>723901</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>530088</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>81998</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>530088</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>158198</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2522,23 +2991,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>33131</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>33131</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323436</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2546,7 +3028,50 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552036</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2818,10 +3343,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V25" sqref="T22:V25"/>
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,87 +3359,51 @@
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="J1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="J4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -2934,30 +3426,8 @@
       <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2982,18 +3452,8 @@
       <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -3018,18 +3478,8 @@
       <c r="H7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3054,18 +3504,8 @@
       <c r="H8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -3090,16 +3530,8 @@
       <c r="H9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -3124,16 +3556,8 @@
       <c r="H10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -3158,18 +3582,8 @@
       <c r="H11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -3194,76 +3608,40 @@
       <c r="H12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="J13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
@@ -3286,28 +3664,6 @@
       <c r="H16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="4" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -3334,264 +3690,144 @@
       <c r="H17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="T22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N22" s="14" t="s">
+      <c r="U22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="O22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="P22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="U22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="V22" s="14" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="9">
         <v>25263</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="9">
         <v>34341</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="9">
         <v>70132</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="9">
         <v>20921</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="9">
         <v>19341</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="9">
         <v>17763</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="9">
         <v>46973</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="T23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="15">
-        <v>2444</v>
-      </c>
-      <c r="L23" s="15">
-        <v>7331</v>
-      </c>
-      <c r="M23" s="15">
-        <v>11869</v>
-      </c>
-      <c r="N23" s="15">
+      <c r="U23" s="12">
+        <v>5249</v>
+      </c>
+      <c r="V23" s="12">
         <v>51096</v>
       </c>
-      <c r="O23" s="15">
-        <v>5249</v>
-      </c>
-      <c r="P23" s="15">
-        <v>4619</v>
-      </c>
-      <c r="Q23" s="15">
-        <v>2094</v>
-      </c>
-      <c r="T23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="U23" s="15">
-        <v>5249</v>
-      </c>
-      <c r="V23" s="15">
-        <v>51096</v>
-      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="9">
         <v>35526</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>104208</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="9">
         <v>95791</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="9">
         <v>6710</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="9">
         <v>5132</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="9">
         <v>5921</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="9">
         <v>32368</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="T24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K24" s="15">
-        <v>2444</v>
-      </c>
-      <c r="L24" s="15">
-        <v>20946</v>
-      </c>
-      <c r="M24" s="15">
-        <v>29324</v>
-      </c>
-      <c r="N24" s="15">
+      <c r="U24" s="12">
+        <v>17148</v>
+      </c>
+      <c r="V24" s="12">
         <v>652688</v>
       </c>
-      <c r="O24" s="15">
-        <v>17148</v>
-      </c>
-      <c r="P24" s="15">
-        <v>5132</v>
-      </c>
-      <c r="Q24" s="15">
-        <v>1746</v>
-      </c>
-      <c r="T24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U24" s="15">
-        <v>17148</v>
-      </c>
-      <c r="V24" s="15">
-        <v>652688</v>
-      </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="9">
         <v>105392</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="9">
         <v>48157</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="9">
         <v>595270</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="9">
         <v>20131</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="9">
         <v>19737</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="9">
         <v>16184</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="9">
         <v>29605</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="T25" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K25" s="15">
-        <v>12567</v>
-      </c>
-      <c r="L25" s="15">
-        <v>504787</v>
-      </c>
-      <c r="M25" s="15">
-        <v>352932</v>
-      </c>
-      <c r="N25" s="15">
-        <v>1028901</v>
-      </c>
-      <c r="O25" s="15">
+      <c r="U25" s="12">
         <v>43745</v>
       </c>
-      <c r="P25" s="15">
-        <v>21553</v>
-      </c>
-      <c r="Q25" s="15">
-        <v>15360</v>
-      </c>
-      <c r="T25" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U25" s="15">
-        <v>43745</v>
-      </c>
-      <c r="V25" s="15">
+      <c r="V25" s="12">
         <v>1028901</v>
       </c>
     </row>
@@ -3599,16 +3835,703 @@
       <c r="S30" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A1:H3"/>
     <mergeCell ref="A13:H15"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="J1:Q3"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="J13:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H25" sqref="A1:H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="17">
+        <v>2444</v>
+      </c>
+      <c r="C23" s="17">
+        <v>7331</v>
+      </c>
+      <c r="D23" s="17">
+        <v>11869</v>
+      </c>
+      <c r="E23" s="17">
+        <v>51096</v>
+      </c>
+      <c r="F23" s="17">
+        <v>5249</v>
+      </c>
+      <c r="G23" s="17">
+        <v>4619</v>
+      </c>
+      <c r="H23" s="17">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="17">
+        <v>2444</v>
+      </c>
+      <c r="C24" s="17">
+        <v>20946</v>
+      </c>
+      <c r="D24" s="17">
+        <v>29324</v>
+      </c>
+      <c r="E24" s="17">
+        <v>652688</v>
+      </c>
+      <c r="F24" s="17">
+        <v>17148</v>
+      </c>
+      <c r="G24" s="17">
+        <v>5132</v>
+      </c>
+      <c r="H24" s="17">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="17">
+        <v>12567</v>
+      </c>
+      <c r="C25" s="17">
+        <v>504787</v>
+      </c>
+      <c r="D25" s="17">
+        <v>352932</v>
+      </c>
+      <c r="E25" s="17">
+        <v>1028901</v>
+      </c>
+      <c r="F25" s="17">
+        <v>43745</v>
+      </c>
+      <c r="G25" s="17">
+        <v>21553</v>
+      </c>
+      <c r="H25" s="17">
+        <v>15360</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A13:H15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="17">
+        <v>36046</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="17">
+        <v>266324</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="17">
+        <v>1245531</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A13:H15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se modifican documentos de conclusiones y resumen
</commit_message>
<xml_diff>
--- a/ResumenDePruebasYComplejidadComputacional.xlsx
+++ b/ResumenDePruebasYComplejidadComputacional.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceYanina\PruebasParaElTP2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="POLINOMIO" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="BINOMIO DE NEWTON DESARROLLADO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="24">
   <si>
     <t>Grado 0</t>
   </si>
@@ -103,8 +98,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +318,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,12 +331,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -357,17 +352,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -451,7 +436,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -460,13 +444,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -490,7 +472,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>POLINOMIO!$B$22:$H$22</c:f>
@@ -579,7 +560,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>POLINOMIO!$B$22:$H$22</c:f>
@@ -668,7 +648,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>POLINOMIO!$B$22:$H$22</c:f>
@@ -734,28 +713,18 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="331190056"/>
-        <c:axId val="331196328"/>
+        <c:axId val="55107968"/>
+        <c:axId val="55109504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="331190056"/>
+        <c:axId val="55107968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -787,22 +756,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331196328"/>
+        <c:crossAx val="55109504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="331196328"/>
+        <c:axId val="55109504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -820,7 +787,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -846,10 +812,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331190056"/>
+        <c:crossAx val="55107968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -864,7 +830,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -889,13 +854,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -919,12 +883,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -932,17 +896,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -951,7 +905,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="es-ES" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -980,10 +934,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.14288188976377952"/>
-          <c:y val="4.6296296296296294E-3"/>
+          <c:y val="4.6296296296296311E-3"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -991,33 +944,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1091,7 +1022,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1166,25 +1096,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="331194368"/>
-        <c:axId val="331194760"/>
+        <c:axId val="56700928"/>
+        <c:axId val="56702848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="331194368"/>
+        <c:axId val="56700928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1201,7 +1121,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1221,7 +1140,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1233,19 +1152,18 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331194760"/>
+        <c:crossAx val="56702848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="331194760"/>
+        <c:axId val="56702848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1263,7 +1181,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1283,7 +1200,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1295,10 +1212,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331194368"/>
+        <c:crossAx val="56700928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1312,8 +1229,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1326,7 +1241,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1338,13 +1253,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1368,12 +1282,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1381,17 +1295,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1445,10 +1349,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.28645303738146932"/>
-          <c:y val="9.937886902673658E-3"/>
+          <c:y val="9.9378869026736649E-3"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1457,13 +1360,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1478,7 +1379,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'BINOMIO DE NEWTON'!$B$22:$H$22</c:f>
@@ -1558,7 +1458,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'BINOMIO DE NEWTON'!$B$22:$H$22</c:f>
@@ -1638,7 +1537,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'BINOMIO DE NEWTON'!$B$22:$H$22</c:f>
@@ -1704,28 +1602,18 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="381338832"/>
-        <c:axId val="381341184"/>
+        <c:axId val="52087808"/>
+        <c:axId val="52097792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="381338832"/>
+        <c:axId val="52087808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1757,22 +1645,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381341184"/>
+        <c:crossAx val="52097792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381341184"/>
+        <c:axId val="52097792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1790,7 +1676,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1816,10 +1701,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381338832"/>
+        <c:crossAx val="52087808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1834,7 +1719,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1859,13 +1743,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1889,12 +1772,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1902,17 +1785,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1966,10 +1839,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.28645303738146932"/>
-          <c:y val="9.937886902673658E-3"/>
+          <c:y val="9.9378869026736649E-3"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1978,13 +1850,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1999,7 +1869,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$22:$H$22</c:f>
@@ -2061,7 +1930,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$22:$H$22</c:f>
@@ -2123,7 +1991,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'BINOMIO DE NEWTON DESARROLLADO'!$B$22:$H$22</c:f>
@@ -2171,28 +2038,18 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="332302544"/>
-        <c:axId val="382465464"/>
+        <c:axId val="53702016"/>
+        <c:axId val="54871168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="332302544"/>
+        <c:axId val="53702016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2224,22 +2081,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382465464"/>
+        <c:crossAx val="54871168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="382465464"/>
+        <c:axId val="54871168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2257,7 +2112,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2283,10 +2137,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332302544"/>
+        <c:crossAx val="53702016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2300,8 +2154,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2326,13 +2178,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2356,12 +2207,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3335,75 +3186,75 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -3427,7 +3278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3453,7 +3304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -3479,7 +3330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3505,7 +3356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -3531,7 +3382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -3557,7 +3408,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -3583,7 +3434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -3609,39 +3460,39 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
@@ -3665,7 +3516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -3691,7 +3542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
@@ -3726,7 +3577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
@@ -3761,7 +3612,7 @@
         <v>51096</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
@@ -3796,7 +3647,7 @@
         <v>652688</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="7" t="s">
         <v>20</v>
       </c>
@@ -3831,7 +3682,7 @@
         <v>1028901</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="S30" s="6"/>
     </row>
   </sheetData>
@@ -3847,66 +3698,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H25" sqref="A1:H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -3930,119 +3781,221 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
@@ -4066,7 +4019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -4092,8 +4045,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -4118,81 +4071,81 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="14">
         <v>2444</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="14">
         <v>7331</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="14">
         <v>11869</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="14">
         <v>51096</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="14">
         <v>5249</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="14">
         <v>4619</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="14">
         <v>2094</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="14">
         <v>2444</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="14">
         <v>20946</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="14">
         <v>29324</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="14">
         <v>652688</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="14">
         <v>17148</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="14">
         <v>5132</v>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="14">
         <v>1746</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="14">
         <v>12567</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="14">
         <v>504787</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="14">
         <v>352932</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="14">
         <v>1028901</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="14">
         <v>43745</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="14">
         <v>21553</v>
       </c>
-      <c r="H25" s="17">
+      <c r="H25" s="14">
         <v>15360</v>
       </c>
     </row>
@@ -4209,66 +4162,66 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -4292,7 +4245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -4304,7 +4257,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -4316,7 +4269,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -4328,7 +4281,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
@@ -4338,7 +4291,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
@@ -4348,7 +4301,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -4360,7 +4313,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -4372,39 +4325,39 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
@@ -4428,7 +4381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -4454,8 +4407,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:11">
+      <c r="A22" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -4480,49 +4433,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="14">
         <v>36046</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="14">
         <v>266324</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="14">
         <v>1245531</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:11">
       <c r="K26" s="6"/>
     </row>
   </sheetData>

</xml_diff>